<commit_message>
增加工作SQL Signed-off-by: 59471740@qq.com <59471740@qq.com>
</commit_message>
<xml_diff>
--- a/evm_doc/项目功能变更历史.xlsx
+++ b/evm_doc/项目功能变更历史.xlsx
@@ -2884,7 +2884,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{733e8537-237e-48f3-afe0-1698189c47b6}</x14:id>
+          <x14:id>{ba462392-bc9f-4b7d-82ea-30b30fbeb2eb}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2898,7 +2898,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{a15f9545-5729-46b1-a358-dca267c72276}</x14:id>
+          <x14:id>{37ac8e1d-c336-4cc2-9cf5-845ed53490b9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2915,7 +2915,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b1597c0a-7524-41af-b0e4-be2488ccb4f7}</x14:id>
+          <x14:id>{e1b11c2c-06c1-436d-87bf-ae711c1e6cec}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2932,7 +2932,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0776695c-9a81-43cd-900a-27cce5702581}</x14:id>
+          <x14:id>{c4387f85-73b1-469e-a720-8291486770d9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2954,7 +2954,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{03006a72-4650-44b2-a918-af0a79a0cacb}</x14:id>
+          <x14:id>{41ed3d24-4db1-456b-8558-4e2bfa64268b}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2968,7 +2968,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3d9271e1-5501-4a1f-8bf1-867c19493352}</x14:id>
+          <x14:id>{9b6849fc-1ab1-4e2b-9fb8-29ebbf1c84c2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2982,7 +2982,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{df4ad382-2a60-4ef6-90d5-968d52afe1f7}</x14:id>
+          <x14:id>{75d1afe4-e4c5-4e5b-bf41-f1cd0f6627f1}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2995,7 +2995,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{733e8537-237e-48f3-afe0-1698189c47b6}">
+          <x14:cfRule type="dataBar" id="{ba462392-bc9f-4b7d-82ea-30b30fbeb2eb}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3008,7 +3008,7 @@
           <xm:sqref>C65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{a15f9545-5729-46b1-a358-dca267c72276}">
+          <x14:cfRule type="dataBar" id="{37ac8e1d-c336-4cc2-9cf5-845ed53490b9}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3021,7 +3021,7 @@
           <xm:sqref>C119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b1597c0a-7524-41af-b0e4-be2488ccb4f7}">
+          <x14:cfRule type="dataBar" id="{e1b11c2c-06c1-436d-87bf-ae711c1e6cec}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3034,7 +3034,7 @@
           <xm:sqref>C120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0776695c-9a81-43cd-900a-27cce5702581}">
+          <x14:cfRule type="dataBar" id="{c4387f85-73b1-469e-a720-8291486770d9}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3047,7 +3047,7 @@
           <xm:sqref>C122</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{03006a72-4650-44b2-a918-af0a79a0cacb}">
+          <x14:cfRule type="dataBar" id="{41ed3d24-4db1-456b-8558-4e2bfa64268b}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3060,7 +3060,7 @@
           <xm:sqref>C2:C45 C48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3d9271e1-5501-4a1f-8bf1-867c19493352}">
+          <x14:cfRule type="dataBar" id="{9b6849fc-1ab1-4e2b-9fb8-29ebbf1c84c2}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -3073,7 +3073,7 @@
           <xm:sqref>C56:C64 C49:C54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{df4ad382-2a60-4ef6-90d5-968d52afe1f7}">
+          <x14:cfRule type="dataBar" id="{75d1afe4-e4c5-4e5b-bf41-f1cd0f6627f1}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>